<commit_message>
Labs made before 14.09.2024
</commit_message>
<xml_diff>
--- a/Лабы.xlsx
+++ b/Лабы.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F69FE5-6539-4BDC-9D1E-41E0C0560240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23632D6A-9149-434A-8FEC-1AF3AE86B537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -131,11 +131,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K6:K8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -493,12 +493,12 @@
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -513,7 +513,7 @@
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="3"/>
+      <c r="B3" s="7"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -536,7 +536,7 @@
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="3"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -557,9 +557,9 @@
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -575,7 +575,7 @@
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="4"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -596,7 +596,7 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>

</xml_diff>

<commit_message>
Labs made before 29.09.2024
</commit_message>
<xml_diff>
--- a/Лабы.xlsx
+++ b/Лабы.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC1447A-445B-4394-B8E3-EA7C7EB4EA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E29F48-77BF-4087-AF43-51C3007C99B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -136,6 +136,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -419,7 +420,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -499,8 +500,8 @@
       <c r="E2" s="4"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="1"/>
@@ -516,7 +517,7 @@
       <c r="B3" s="7"/>
       <c r="C3" s="6"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="3"/>
+      <c r="E3" s="5"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -525,12 +526,12 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -539,7 +540,7 @@
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5"/>
-      <c r="E4" s="1"/>
+      <c r="E4" s="3"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -563,7 +564,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="1"/>
+      <c r="H5" s="3"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -578,7 +579,7 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="6"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
@@ -590,11 +591,11 @@
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>

</xml_diff>

<commit_message>
Labs made before 07.10.2024
</commit_message>
<xml_diff>
--- a/Лабы.xlsx
+++ b/Лабы.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E29F48-77BF-4087-AF43-51C3007C99B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54A33D1-FF06-4BE3-B78A-B5712A41F242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -136,7 +136,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -420,7 +419,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,9 +515,9 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="6"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="3"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -526,12 +525,6 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="8"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -539,9 +532,9 @@
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="3"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -580,7 +573,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -594,9 +587,9 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -608,9 +601,9 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
+      <c r="D8" s="6"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -622,8 +615,8 @@
         <v>8</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="3"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>

</xml_diff>

<commit_message>
Labs made before 17.10.2024
</commit_message>
<xml_diff>
--- a/Лабы.xlsx
+++ b/Лабы.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28213"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54A33D1-FF06-4BE3-B78A-B5712A41F242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71D0D8F-B3B9-4D44-AF49-9FEE141D9274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +501,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="3"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="3"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -517,8 +517,8 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="1"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="3"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -534,8 +534,8 @@
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="1"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="3"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -558,7 +558,7 @@
       <c r="F5" s="6"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="I5" s="1"/>
+      <c r="I5" s="3"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -573,8 +573,8 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="3"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -589,10 +589,10 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="3"/>
       <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -604,7 +604,7 @@
       <c r="D8" s="6"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="3"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -626,7 +626,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="1"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>

</xml_diff>

<commit_message>
Labs made before 01.11.2024
</commit_message>
<xml_diff>
--- a/Лабы.xlsx
+++ b/Лабы.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28221"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F71D0D8F-B3B9-4D44-AF49-9FEE141D9274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F49362-A4D9-4A7A-A46A-425100AE1013}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +76,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -136,6 +143,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -419,7 +428,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="D9" sqref="B9:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -501,7 +510,7 @@
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="5"/>
+      <c r="J2" s="6"/>
       <c r="K2" s="3"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -518,13 +527,16 @@
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="5"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="3"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -535,8 +547,8 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -559,11 +571,14 @@
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -574,11 +589,16 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="3"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -594,6 +614,11 @@
       <c r="I7" s="6"/>
       <c r="J7" s="3"/>
       <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
@@ -602,24 +627,31 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="3"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -627,8 +659,8 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>

</xml_diff>

<commit_message>
Labs made before 21.11.2024
</commit_message>
<xml_diff>
--- a/Лабы.xlsx
+++ b/Лабы.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF45640-A3C6-4F9A-8C47-FB735FCCF142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BB13E4-DED0-4A49-B884-E1572139C69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="B10:E10"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,8 +568,8 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="1"/>
@@ -627,7 +627,7 @@
       <c r="F8" s="8"/>
       <c r="G8" s="6"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="1"/>
+      <c r="I8" s="3"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>

</xml_diff>